<commit_message>
Added data for Pb ads experiments
</commit_message>
<xml_diff>
--- a/Regression/Kinetics/data/klebsiella_living_v_dead.xlsx
+++ b/Regression/Kinetics/data/klebsiella_living_v_dead.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="10">
   <si>
     <t xml:space="preserve">Bottle number</t>
   </si>
@@ -163,11 +163,11 @@
   </sheetPr>
   <dimension ref="A1:G55"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A32" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F56" activeCellId="0" sqref="F56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="2.57"/>
@@ -212,7 +212,9 @@
       <c r="E2" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="F2" s="2"/>
+      <c r="F2" s="2" t="n">
+        <v>5.15</v>
+      </c>
       <c r="G2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -231,7 +233,9 @@
       <c r="E3" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="F3" s="2"/>
+      <c r="F3" s="2" t="n">
+        <v>5.306</v>
+      </c>
       <c r="G3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -250,7 +254,9 @@
       <c r="E4" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="F4" s="2"/>
+      <c r="F4" s="2" t="n">
+        <v>5.3</v>
+      </c>
       <c r="G4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -269,7 +275,9 @@
       <c r="E5" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="F5" s="2"/>
+      <c r="F5" s="2" t="n">
+        <v>5.782</v>
+      </c>
       <c r="G5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -288,7 +296,9 @@
       <c r="E6" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="F6" s="2"/>
+      <c r="F6" s="2" t="n">
+        <v>5.904</v>
+      </c>
       <c r="G6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -307,7 +317,9 @@
       <c r="E7" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="F7" s="2"/>
+      <c r="F7" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="G7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -326,7 +338,9 @@
       <c r="E8" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="F8" s="2"/>
+      <c r="F8" s="2" t="n">
+        <v>5.15</v>
+      </c>
       <c r="G8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -345,7 +359,9 @@
       <c r="E9" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="F9" s="2"/>
+      <c r="F9" s="2" t="n">
+        <v>6.029</v>
+      </c>
       <c r="G9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -364,7 +380,9 @@
       <c r="E10" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="F10" s="2"/>
+      <c r="F10" s="2" t="n">
+        <v>5.756</v>
+      </c>
       <c r="G10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -383,7 +401,9 @@
       <c r="E11" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="F11" s="2"/>
+      <c r="F11" s="2" t="n">
+        <v>6.08</v>
+      </c>
       <c r="G11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -402,7 +422,9 @@
       <c r="E12" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="F12" s="2"/>
+      <c r="F12" s="2" t="n">
+        <v>6.084</v>
+      </c>
       <c r="G12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -421,7 +443,9 @@
       <c r="E13" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="F13" s="2"/>
+      <c r="F13" s="2" t="n">
+        <v>5.914</v>
+      </c>
       <c r="G13" s="2"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -440,7 +464,9 @@
       <c r="E14" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="F14" s="2"/>
+      <c r="F14" s="2" t="n">
+        <v>5.15</v>
+      </c>
       <c r="G14" s="2"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -459,7 +485,9 @@
       <c r="E15" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="F15" s="2"/>
+      <c r="F15" s="2" t="n">
+        <v>5.757</v>
+      </c>
       <c r="G15" s="2"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -478,7 +506,9 @@
       <c r="E16" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="F16" s="2"/>
+      <c r="F16" s="2" t="n">
+        <v>5.71</v>
+      </c>
       <c r="G16" s="2"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -497,7 +527,9 @@
       <c r="E17" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="F17" s="2"/>
+      <c r="F17" s="2" t="n">
+        <v>5.98</v>
+      </c>
       <c r="G17" s="2"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -516,7 +548,9 @@
       <c r="E18" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="F18" s="2"/>
+      <c r="F18" s="2" t="n">
+        <v>5.829</v>
+      </c>
       <c r="G18" s="2"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -535,7 +569,9 @@
       <c r="E19" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="F19" s="2"/>
+      <c r="F19" s="2" t="n">
+        <v>5.283</v>
+      </c>
       <c r="G19" s="2"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -554,7 +590,9 @@
       <c r="E20" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="F20" s="2"/>
+      <c r="F20" s="2" t="n">
+        <v>5.01</v>
+      </c>
       <c r="G20" s="2"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -573,7 +611,9 @@
       <c r="E21" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="F21" s="2"/>
+      <c r="F21" s="2" t="n">
+        <v>5.06</v>
+      </c>
       <c r="G21" s="2"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -592,7 +632,9 @@
       <c r="E22" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="F22" s="2"/>
+      <c r="F22" s="2" t="n">
+        <v>5.101</v>
+      </c>
       <c r="G22" s="2"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -611,7 +653,9 @@
       <c r="E23" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="F23" s="2"/>
+      <c r="F23" s="2" t="n">
+        <v>4.594</v>
+      </c>
       <c r="G23" s="2"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -630,7 +674,9 @@
       <c r="E24" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="F24" s="2"/>
+      <c r="F24" s="2" t="n">
+        <v>4.932</v>
+      </c>
       <c r="G24" s="2"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -649,7 +695,9 @@
       <c r="E25" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="F25" s="2"/>
+      <c r="F25" s="2" t="n">
+        <v>5.291</v>
+      </c>
       <c r="G25" s="2"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -668,7 +716,9 @@
       <c r="E26" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="F26" s="2"/>
+      <c r="F26" s="2" t="n">
+        <v>5.01</v>
+      </c>
       <c r="G26" s="2"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -687,7 +737,9 @@
       <c r="E27" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="F27" s="2"/>
+      <c r="F27" s="2" t="n">
+        <v>5.229</v>
+      </c>
       <c r="G27" s="2"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -706,7 +758,9 @@
       <c r="E28" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="F28" s="2"/>
+      <c r="F28" s="2" t="n">
+        <v>4.834</v>
+      </c>
       <c r="G28" s="2"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -725,7 +779,9 @@
       <c r="E29" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="F29" s="2"/>
+      <c r="F29" s="2" t="n">
+        <v>5.279</v>
+      </c>
       <c r="G29" s="2"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -744,7 +800,9 @@
       <c r="E30" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="F30" s="2"/>
+      <c r="F30" s="2" t="n">
+        <v>5.378</v>
+      </c>
       <c r="G30" s="2"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -763,7 +821,9 @@
       <c r="E31" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="F31" s="2"/>
+      <c r="F31" s="2" t="n">
+        <v>5</v>
+      </c>
       <c r="G31" s="2"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -782,7 +842,9 @@
       <c r="E32" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="F32" s="2"/>
+      <c r="F32" s="2" t="n">
+        <v>5.01</v>
+      </c>
       <c r="G32" s="2"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -801,7 +863,9 @@
       <c r="E33" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="F33" s="2"/>
+      <c r="F33" s="2" t="n">
+        <v>5.321</v>
+      </c>
       <c r="G33" s="2"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -820,7 +884,9 @@
       <c r="E34" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="F34" s="2"/>
+      <c r="F34" s="2" t="n">
+        <v>5.109</v>
+      </c>
       <c r="G34" s="2"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -839,7 +905,9 @@
       <c r="E35" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="F35" s="2"/>
+      <c r="F35" s="2" t="n">
+        <v>5.188</v>
+      </c>
       <c r="G35" s="2"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -858,7 +926,9 @@
       <c r="E36" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="F36" s="2"/>
+      <c r="F36" s="2" t="n">
+        <v>5.136</v>
+      </c>
       <c r="G36" s="2"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -877,7 +947,9 @@
       <c r="E37" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="F37" s="2"/>
+      <c r="F37" s="2" t="n">
+        <v>4.942</v>
+      </c>
       <c r="G37" s="2"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -896,7 +968,9 @@
       <c r="E38" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="F38" s="2"/>
+      <c r="F38" s="2" t="n">
+        <v>5.05</v>
+      </c>
       <c r="G38" s="2"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -915,7 +989,9 @@
       <c r="E39" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="F39" s="2"/>
+      <c r="F39" s="2" t="n">
+        <v>4.782</v>
+      </c>
       <c r="G39" s="2"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -934,7 +1010,9 @@
       <c r="E40" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="F40" s="2"/>
+      <c r="F40" s="2" t="n">
+        <v>4.946</v>
+      </c>
       <c r="G40" s="2"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -953,7 +1031,9 @@
       <c r="E41" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="F41" s="2"/>
+      <c r="F41" s="2" t="n">
+        <v>5.253</v>
+      </c>
       <c r="G41" s="2"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -972,7 +1052,9 @@
       <c r="E42" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="F42" s="2"/>
+      <c r="F42" s="2" t="n">
+        <v>5.199</v>
+      </c>
       <c r="G42" s="2"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -991,7 +1073,9 @@
       <c r="E43" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="F43" s="2"/>
+      <c r="F43" s="2" t="n">
+        <v>4.954</v>
+      </c>
       <c r="G43" s="2"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1010,7 +1094,9 @@
       <c r="E44" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="F44" s="2"/>
+      <c r="F44" s="2" t="n">
+        <v>5.05</v>
+      </c>
       <c r="G44" s="2"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1029,7 +1115,9 @@
       <c r="E45" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="F45" s="2"/>
+      <c r="F45" s="2" t="n">
+        <v>5.068</v>
+      </c>
       <c r="G45" s="2"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1048,7 +1136,9 @@
       <c r="E46" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="F46" s="2"/>
+      <c r="F46" s="2" t="n">
+        <v>5.132</v>
+      </c>
       <c r="G46" s="2"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1067,7 +1157,9 @@
       <c r="E47" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="F47" s="2"/>
+      <c r="F47" s="2" t="n">
+        <v>5.146</v>
+      </c>
       <c r="G47" s="2"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1086,7 +1178,9 @@
       <c r="E48" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="F48" s="2"/>
+      <c r="F48" s="2" t="n">
+        <v>5.27</v>
+      </c>
       <c r="G48" s="2"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1105,7 +1199,9 @@
       <c r="E49" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="F49" s="2"/>
+      <c r="F49" s="2" t="n">
+        <v>4.873</v>
+      </c>
       <c r="G49" s="2"/>
     </row>
     <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1124,6 +1220,9 @@
       <c r="E50" s="2" t="n">
         <v>10</v>
       </c>
+      <c r="F50" s="0" t="n">
+        <v>5.05</v>
+      </c>
     </row>
     <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="n">
@@ -1141,6 +1240,9 @@
       <c r="E51" s="2" t="n">
         <v>10</v>
       </c>
+      <c r="F51" s="0" t="n">
+        <v>4.84</v>
+      </c>
     </row>
     <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="n">
@@ -1158,6 +1260,9 @@
       <c r="E52" s="2" t="n">
         <v>10</v>
       </c>
+      <c r="F52" s="0" t="n">
+        <v>5.315</v>
+      </c>
     </row>
     <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="n">
@@ -1175,6 +1280,9 @@
       <c r="E53" s="2" t="n">
         <v>10</v>
       </c>
+      <c r="F53" s="0" t="n">
+        <v>5.109</v>
+      </c>
     </row>
     <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="n">
@@ -1192,6 +1300,9 @@
       <c r="E54" s="2" t="n">
         <v>10</v>
       </c>
+      <c r="F54" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="n">
@@ -1208,6 +1319,9 @@
       </c>
       <c r="E55" s="2" t="n">
         <v>10</v>
+      </c>
+      <c r="F55" s="0" t="n">
+        <v>4.972</v>
       </c>
     </row>
   </sheetData>

</xml_diff>